<commit_message>
94.6% test accuracy check in and clean up
</commit_message>
<xml_diff>
--- a/TrialData.xlsx
+++ b/TrialData.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usshajoe\Desktop\MachineLearning\CarND_Project2_Traffic_Signs\CarND_Project2_Traffic_Signs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="75" windowWidth="16215" windowHeight="5910"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="54">
   <si>
     <t>Trial #</t>
   </si>
@@ -160,13 +165,31 @@
   </si>
   <si>
     <t>768,43</t>
+  </si>
+  <si>
+    <t>Generator, No Balancing, 50% augmentation</t>
+  </si>
+  <si>
+    <t>5,5,6,20</t>
+  </si>
+  <si>
+    <t>250,43</t>
+  </si>
+  <si>
+    <t>5,5,6,18</t>
+  </si>
+  <si>
+    <t>5,5,18,27</t>
+  </si>
+  <si>
+    <t>243,43</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -174,13 +197,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -195,9 +230,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -258,7 +295,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -290,9 +327,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -324,6 +362,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -499,16 +538,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,7 +612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -632,7 +671,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -691,7 +730,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -753,7 +792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -815,7 +854,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -877,7 +916,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -945,7 +984,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1004,7 +1043,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1066,18 +1105,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
+      <c r="B10">
+        <v>74.2</v>
+      </c>
+      <c r="C10">
+        <v>76.8</v>
+      </c>
+      <c r="D10">
+        <v>84.4</v>
       </c>
       <c r="E10" t="s">
         <v>39</v>
@@ -1128,7 +1167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1193,7 +1232,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1258,7 +1297,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1320,7 +1359,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1385,10 +1424,19 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15">
+        <v>87.3</v>
+      </c>
+      <c r="C15">
+        <v>88.9</v>
+      </c>
+      <c r="D15">
+        <v>98.9</v>
+      </c>
       <c r="E15" t="s">
         <v>44</v>
       </c>
@@ -1417,7 +1465,7 @@
         <v>1E-3</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="P15">
         <v>512</v>
@@ -1438,33 +1486,224 @@
         <v>43</v>
       </c>
       <c r="V15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>92.4</v>
+      </c>
+      <c r="C16">
+        <v>92.3</v>
+      </c>
+      <c r="D16">
+        <v>99.9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>4</v>
+      </c>
+      <c r="K16" s="1">
+        <v>400120</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N16">
+        <v>1E-3</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>512</v>
+      </c>
+      <c r="Q16">
+        <v>40</v>
+      </c>
+      <c r="R16" t="s">
+        <v>23</v>
+      </c>
+      <c r="S16" t="s">
+        <v>15</v>
+      </c>
+      <c r="T16" t="s">
+        <v>48</v>
+      </c>
+      <c r="U16" t="s">
+        <v>43</v>
+      </c>
+      <c r="V16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>94</v>
+      </c>
+      <c r="C17">
+        <v>94.5</v>
+      </c>
+      <c r="D17">
+        <v>99.8</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" t="s">
+        <v>4</v>
+      </c>
+      <c r="K17" s="1">
+        <v>500500</v>
+      </c>
+      <c r="L17" s="1">
+        <v>500250</v>
+      </c>
+      <c r="M17" t="s">
+        <v>50</v>
+      </c>
+      <c r="N17">
+        <v>1E-3</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>512</v>
+      </c>
+      <c r="Q17">
+        <v>40</v>
+      </c>
+      <c r="R17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" t="s">
+        <v>15</v>
+      </c>
+      <c r="T17" t="s">
+        <v>48</v>
+      </c>
+      <c r="U17" t="s">
+        <v>43</v>
+      </c>
+      <c r="V17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>94.6</v>
+      </c>
+      <c r="C18" s="2">
+        <v>95.6</v>
+      </c>
+      <c r="D18" s="2">
+        <v>99.6</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K18" s="3">
+        <v>243243</v>
+      </c>
+      <c r="L18" s="3">
+        <v>243243</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+      <c r="P18" s="2">
+        <v>512</v>
+      </c>
+      <c r="Q18" s="2">
+        <v>40</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="V18" s="2" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>